<commit_message>
Fixed issue with the game over screen not triggering on second enemy hit Jira_Id - RWMPA22-103
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gameuser\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gameuser\Desktop\Temp2.0\RWM-Endless-Jumper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D308C71-8A91-4B00-8955-58BD8E3E4559}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13AE424F-4345-4AF0-ABE2-26552CE33530}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>JIRA</t>
   </si>
@@ -350,7 +350,7 @@
   <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Fixed issue with the game over screen not triggering on second enemy hit Jira_Id - RWMPA22-103 (#9)
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gameuser\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gameuser\Desktop\Temp2.0\RWM-Endless-Jumper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D308C71-8A91-4B00-8955-58BD8E3E4559}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13AE424F-4345-4AF0-ABE2-26552CE33530}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>JIRA</t>
   </si>
@@ -350,7 +350,7 @@
   <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added hurt particle effect RWMPA22-93
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gameuser\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gameuser\Desktop\Temp2.0\RWM-Endless-Jumper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D308C71-8A91-4B00-8955-58BD8E3E4559}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13AE424F-4345-4AF0-ABE2-26552CE33530}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>JIRA</t>
   </si>
@@ -350,7 +350,7 @@
   <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>